<commit_message>
adjust graphs after data integration
</commit_message>
<xml_diff>
--- a/data/commitments_pillars_goals.xlsx
+++ b/data/commitments_pillars_goals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/digilateral/Dropbox/Patryk/Digilateral/GIFI/DFI Tracker/Data Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D26F2F8-7CAD-4395-AF95-0167AF0A34B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7C52F3B-2101-45FC-B299-E999AB1134EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="1900" windowWidth="28360" windowHeight="12060" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,7 +156,7 @@
     <t>goal_num</t>
   </si>
   <si>
-    <t>goal_text</t>
+    <t>goal_txt</t>
   </si>
   <si>
     <t>goal_txt_short</t>
@@ -722,7 +722,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="pillar_txt"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="pillar_txt_short"/>
     <tableColumn id="6" xr3:uid="{DF16E977-A8CA-3248-A196-F27EB897C5E0}" name="goal_num"/>
-    <tableColumn id="7" xr3:uid="{1802A717-C184-3142-9EE9-E5D145FFC398}" name="goal_text"/>
+    <tableColumn id="7" xr3:uid="{1802A717-C184-3142-9EE9-E5D145FFC398}" name="goal_txt"/>
     <tableColumn id="8" xr3:uid="{C0E578DF-B080-BA48-95E4-8663E4DAB798}" name="goal_txt_short"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -933,8 +933,8 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1370,8 +1370,8 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="G2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -2537,6 +2537,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0b45af84-26f8-4e58-b6b2-ac91f42d435d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1d2a751e-c940-49fb-b129-5edb270068eb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E3DD8F6A53105498A3DA392E71453A7" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d601f522e3e51b19c3f9226f134eddba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1d2a751e-c940-49fb-b129-5edb270068eb" xmlns:ns3="0b45af84-26f8-4e58-b6b2-ac91f42d435d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b945da9333134c263560e394374875cf" ns2:_="" ns3:_="">
     <xsd:import namespace="1d2a751e-c940-49fb-b129-5edb270068eb"/>
@@ -2771,28 +2791,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0b45af84-26f8-4e58-b6b2-ac91f42d435d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1d2a751e-c940-49fb-b129-5edb270068eb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C79D2A07-AA8D-47D9-9A7D-BC71B2C7D918}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{965E4D91-83F3-4E83-B9C6-B05C905A3F5F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2800,5 +2800,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{965E4D91-83F3-4E83-B9C6-B05C905A3F5F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C79D2A07-AA8D-47D9-9A7D-BC71B2C7D918}"/>
 </file>
</xml_diff>